<commit_message>
updates for final submission
include sex in source data , change figure names
</commit_message>
<xml_diff>
--- a/data/behav/controlMeasuresDf.xlsx
+++ b/data/behav/controlMeasuresDf.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina Krenz\Documents\GitHub\MemorySemantization\data\behav\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2524E551-D26E-4A98-A9A4-C1C3262A9B2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -19,9 +25,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>delay</t>
   </si>
   <si>
@@ -239,16 +242,19 @@
   </si>
   <si>
     <t>28d</t>
+  </si>
+  <si>
+    <t>sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,15 +314,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -358,7 +372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,9 +404,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,6 +456,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -599,84 +649,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>21</v>
@@ -727,18 +783,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3">
         <v>18</v>
@@ -789,18 +845,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4">
         <v>27</v>
@@ -839,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="2">
-        <v>43518.56944444445</v>
+        <v>43518.569444444453</v>
       </c>
       <c r="R4" s="2">
         <v>43521</v>
@@ -851,18 +907,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5">
         <v>22</v>
@@ -913,18 +969,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6">
         <v>27</v>
@@ -975,18 +1031,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7">
         <v>19</v>
@@ -1037,18 +1093,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8">
         <v>18</v>
@@ -1099,18 +1155,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9">
         <v>23</v>
@@ -1161,18 +1217,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10">
         <v>23</v>
@@ -1223,18 +1279,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11">
         <v>23</v>
@@ -1285,18 +1341,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12">
         <v>27</v>
@@ -1347,18 +1403,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13">
         <v>27</v>
@@ -1409,18 +1465,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14">
         <v>22</v>
@@ -1471,18 +1527,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15">
         <v>21</v>
@@ -1533,18 +1589,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16">
         <v>23</v>
@@ -1595,18 +1651,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17">
         <v>24</v>
@@ -1657,18 +1713,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>33</v>
@@ -1719,18 +1775,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19">
         <v>28</v>
@@ -1781,18 +1837,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>20</v>
@@ -1843,18 +1899,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>29</v>
@@ -1905,18 +1961,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22">
         <v>23</v>
@@ -1967,18 +2023,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23">
         <v>23</v>
@@ -2029,18 +2085,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24">
         <v>24</v>
@@ -2091,18 +2147,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25">
         <v>22</v>
@@ -2153,18 +2209,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
       </c>
       <c r="E26">
         <v>19</v>
@@ -2215,18 +2271,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
       </c>
       <c r="E27">
         <v>23</v>
@@ -2277,18 +2333,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28">
         <v>29</v>
@@ -2339,18 +2395,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -2401,18 +2457,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
         <v>72</v>
-      </c>
-      <c r="D30" t="s">
-        <v>73</v>
       </c>
       <c r="E30">
         <v>27</v>
@@ -2463,18 +2519,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
         <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>73</v>
       </c>
       <c r="E31">
         <v>33</v>
@@ -2525,18 +2581,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>21</v>
@@ -2587,18 +2643,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33">
         <v>22</v>
@@ -2649,18 +2705,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
         <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
       </c>
       <c r="E34">
         <v>23</v>
@@ -2711,18 +2767,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
         <v>72</v>
-      </c>
-      <c r="D35" t="s">
-        <v>73</v>
       </c>
       <c r="E35">
         <v>26</v>
@@ -2773,18 +2829,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36">
         <v>26</v>
@@ -2835,18 +2891,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E37">
         <v>25</v>
@@ -2897,18 +2953,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="s">
         <v>72</v>
-      </c>
-      <c r="D38" t="s">
-        <v>73</v>
       </c>
       <c r="E38">
         <v>25</v>
@@ -2959,18 +3015,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
         <v>72</v>
-      </c>
-      <c r="D39" t="s">
-        <v>73</v>
       </c>
       <c r="E39">
         <v>19</v>
@@ -3021,18 +3077,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40">
         <v>21</v>
@@ -3083,18 +3139,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E41">
         <v>22</v>
@@ -3145,18 +3201,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" t="s">
         <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>73</v>
       </c>
       <c r="E42">
         <v>19</v>
@@ -3207,18 +3263,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
         <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>73</v>
       </c>
       <c r="E43">
         <v>25</v>
@@ -3269,18 +3325,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44">
         <v>25</v>
@@ -3331,18 +3387,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E45">
         <v>27</v>
@@ -3393,18 +3449,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
         <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>73</v>
       </c>
       <c r="E46">
         <v>18</v>
@@ -3455,18 +3511,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
         <v>72</v>
-      </c>
-      <c r="D47" t="s">
-        <v>73</v>
       </c>
       <c r="E47">
         <v>25</v>
@@ -3517,18 +3573,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E48">
         <v>26</v>
@@ -3579,18 +3635,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E49">
         <v>35</v>
@@ -3641,18 +3697,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E50">
         <v>29</v>
@@ -3703,18 +3759,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E51">
         <v>30</v>
@@ -3765,18 +3821,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" t="s">
         <v>72</v>
-      </c>
-      <c r="D52" t="s">
-        <v>73</v>
       </c>
       <c r="E52">
         <v>29</v>
@@ -3827,18 +3883,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E53">
         <v>20</v>

</xml_diff>